<commit_message>
Updating to most recently revised data
</commit_message>
<xml_diff>
--- a/Data/RawData/YPE_Data/YPE_36/Digital Data_YPE36/YPE_Treedata_Plot_36.xlsx
+++ b/Data/RawData/YPE_Data/YPE_36/Digital Data_YPE36/YPE_Treedata_Plot_36.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="qpzODQ44pSqBdFKcyPq5bVB+QWG9q+4Ix440hx/hTpo="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="L1PE1EigAbzeT1hy8H96SfNXpPXh68I2/wzI87w+l/Q="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
   <authors>
     <author/>
   </authors>
@@ -33,7 +33,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mhPaoZ1wS6xOeiS9XR4CNpvHhpECw=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mgmU0FVjPYmddXEio17UeuNwy+ezQ=="/>
     </ext>
   </extLst>
 </comments>
@@ -540,7 +540,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>

</xml_diff>